<commit_message>
fix figures, conjoint EN
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/top_tax_positive.xlsx
+++ b/xlsx/country_comparison/top_tax_positive.xlsx
@@ -12,11 +12,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
+    <t xml:space="preserve">$ bold('All')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ bold('Europe')</t>
+  </si>
+  <si>
     <t xml:space="preserve">France</t>
   </si>
   <si>
@@ -26,25 +32,25 @@
     <t xml:space="preserve">Italy</t>
   </si>
   <si>
+    <t xml:space="preserve">Poland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switzerland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Japan</t>
   </si>
   <si>
-    <t xml:space="preserve">Poland</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saudi Arabia</t>
   </si>
   <si>
-    <t xml:space="preserve">Spain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switzerland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States</t>
+    <t xml:space="preserve">USA</t>
   </si>
   <si>
     <t xml:space="preserve">Supports tax on world top 1% to finance global poverty reduction
@@ -418,75 +424,93 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.599155642549965</v>
+        <v>0.548749204972874</v>
       </c>
       <c r="C2" t="n">
-        <v>0.605535346545386</v>
+        <v>0.612606004275778</v>
       </c>
       <c r="D2" t="n">
-        <v>0.760678239853407</v>
+        <v>0.616724928283738</v>
       </c>
       <c r="E2" t="n">
-        <v>0.444338150049756</v>
+        <v>0.620808072627315</v>
       </c>
       <c r="F2" t="n">
-        <v>0.510999878180732</v>
+        <v>0.75031578480093</v>
       </c>
       <c r="G2" t="n">
-        <v>0.693864994521377</v>
+        <v>0.495076291993524</v>
       </c>
       <c r="H2" t="n">
-        <v>0.603665076505491</v>
+        <v>0.6117343914093</v>
       </c>
       <c r="I2" t="n">
-        <v>0.633704813674124</v>
+        <v>0.554433842033875</v>
       </c>
       <c r="J2" t="n">
-        <v>0.549117152109116</v>
+        <v>0.529872342725065</v>
       </c>
       <c r="K2" t="n">
-        <v>0.418135368479819</v>
+        <v>0.438153093874799</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.677827112481047</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.508222265196169</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.59525228314343</v>
+        <v>0.488009346515533</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5690731820059</v>
+        <v>0.55532380171867</v>
       </c>
       <c r="D3" t="n">
-        <v>0.59469725530132</v>
+        <v>0.588306427984715</v>
       </c>
       <c r="E3" t="n">
-        <v>0.348635187368182</v>
+        <v>0.528389866344171</v>
       </c>
       <c r="F3" t="n">
-        <v>0.538358445510827</v>
+        <v>0.602852192238351</v>
       </c>
       <c r="G3" t="n">
-        <v>0.673983574601438</v>
+        <v>0.547884560154944</v>
       </c>
       <c r="H3" t="n">
-        <v>0.531126971115995</v>
+        <v>0.567216620094722</v>
       </c>
       <c r="I3" t="n">
-        <v>0.342948299877482</v>
+        <v>0.542572051573976</v>
       </c>
       <c r="J3" t="n">
-        <v>0.56759853825918</v>
+        <v>0.360111742646164</v>
       </c>
       <c r="K3" t="n">
-        <v>0.422740683550459</v>
+        <v>0.351009115929929</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.671355992475847</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.447291263751444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>